<commit_message>
Run Time Test Part 2
2 refinery solutions test.
500000 evolutions solutions test.
</commit_message>
<xml_diff>
--- a/MOEA/Results/Run_Time_Survey.xlsx
+++ b/MOEA/Results/Run_Time_Survey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KernInternship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KernInternship\BETO\MOEA\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36C2455-9A36-48C4-A737-EF0B578EA8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEE2F78-F3F1-449F-8F84-6588CB831FA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{3A82AA98-93C5-4EAE-9FFA-1424D5818FC9}"/>
+    <workbookView xWindow="2310" yWindow="1185" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{3A82AA98-93C5-4EAE-9FFA-1424D5818FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Run Time Test County Increase" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Run Time Generations Test" sheetId="3" r:id="rId3"/>
     <sheet name="Run Time Group Test" sheetId="5" r:id="rId4"/>
     <sheet name="Solutions Test" sheetId="4" r:id="rId5"/>
+    <sheet name="Solutions Test 2R" sheetId="6" r:id="rId6"/>
+    <sheet name="Solutions Test 500e" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>time</t>
   </si>
@@ -98,6 +100,12 @@
   </si>
   <si>
     <t>2.037409853935242 minutes</t>
+  </si>
+  <si>
+    <t>IndexError: list index out of range * 2</t>
+  </si>
+  <si>
+    <t>"     "</t>
   </si>
 </sst>
 </file>
@@ -3449,8 +3457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B988482-A6C5-4E9B-98FD-D641D0F90253}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,7 +3992,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4760,7 +4768,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,4 +5396,1290 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2B2F85-D6D0-4134-94F7-E5FA798941B3}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.22150183916091</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.2249194463094</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.2422897497812899</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>100000</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.23033264080683</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>100000</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.2484547257423402</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>100000</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2.2283401131629899</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>100000</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2.2199276804924</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>100000</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2.2139098763465799</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>100000</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2.2341207583745302</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>100000</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.21567876338958</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>100000</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2.24879715840021</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>100000</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2.2253910104433601</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>100000</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2.21644298632939</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>100000</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2.1997706611951102</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>100000</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2.0382752180099399</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>100000</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2.2106166998545298</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>100000</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2.22594201962153</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>100000</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2.2067138711611398</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>100000</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2.1298262000083898</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>100000</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>2.2111257433891298</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>100000</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>2.2086490313212002</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>100000</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2.1915505011876402</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>100000</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2.2142806172370899</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>100000</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2.2093521197636901</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>100000</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2.19695182641347</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>100000</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DDBE8E-0585-40C6-AA26-E9513F41DBF7}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9.6667896072069794</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>500000</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>9.7280933340390501</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>500000</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>9.5902349988619395</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>500000</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>9.4801382223764996</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>500000</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>10.3919533769289</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>500000</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>9.9572776158650704</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>500000</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>10.2472972194353</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>500000</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10.3385367393493</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>500000</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10.0173184076944</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>500000</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9.4315091013908301</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>500000</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>9.7263618071873896</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>500000</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>9.5541455705960594</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>500000</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>9.7663932363192192</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>500000</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>9.4755637248357107</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>500000</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>9.5418282230694995</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>500000</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>9.1715292215347297</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>500000</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>9.1697232246398901</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>500000</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>9.6435184717178295</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>500000</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>9.3667055209477699</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>500000</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>9.4908158381779995</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>500000</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>9.7923512617746997</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>500000</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>9.8082525769869395</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>500000</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>9.6363863786061597</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>500000</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>9.9930347800254804</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>500000</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>9.5963413000106801</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>500000</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>